<commit_message>
new file:   Different file formats pyspark.docx
</commit_message>
<xml_diff>
--- a/fileformat.xlsx
+++ b/fileformat.xlsx
@@ -35,9 +35,6 @@
     <t>Procedure and points to remember</t>
   </si>
   <si>
-    <t>TEXT FILE</t>
-  </si>
-  <si>
     <t>READ</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>//use any codec here org.apache.hadoop.io.compress.(BZip2Codec or GZipCodec or SnappyCodec)</t>
-  </si>
-  <si>
-    <t>SEQUENCE FILE</t>
   </si>
   <si>
     <r>
@@ -98,9 +92,6 @@
     <t>//here rdd is MapPartitionRDD and not the regular pair RDD.</t>
   </si>
   <si>
-    <t>PARQUET FILE</t>
-  </si>
-  <si>
     <t>//use data frame to load the file.</t>
   </si>
   <si>
@@ -122,16 +113,10 @@
     <t>df.write.mode(SaveMode.Overwrite).format("orc") .save(&lt;path to location&gt;)</t>
   </si>
   <si>
-    <t>AVRO FILE</t>
-  </si>
-  <si>
     <t>sqlContext.setConf("spark.sql.avro.compression.codec","snappy") //use snappy, deflate, uncompressed;</t>
   </si>
   <si>
     <t>dataFrame.write.avro(&lt;path to location&gt;);</t>
-  </si>
-  <si>
-    <t>JSON FILE</t>
   </si>
   <si>
     <t>Examples</t>
@@ -179,11 +164,6 @@
     <t>productsRDD.saveAsSequenceFile("productsRDD_seq")</t>
   </si>
   <si>
-    <t>productsRDD.saveAsTextFile("productsRDD")
-hdfs dfs -ls productsRDD
-hdfs dfs -copyToLocal productsRDD/* /home/….</t>
-  </si>
-  <si>
     <t>import com.databricks.spark.avro._;
 sqlContext.read.avro(&lt;path to location&gt;); // this results in a data frame object</t>
   </si>
@@ -191,19 +171,6 @@
     <t xml:space="preserve">spark-shell --packages com.databricks:spark-avro_2.10:2.0.1
 import com.databricks.spark.avro._
 sqlContext.read.avro("orders_result_snappy").show(10)
-</t>
-  </si>
-  <si>
-    <t>sqlContext.setConf("spark.sql.avro.compression.codec","snappy")
-ordersDF.write.avro("orders_result_snappy")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sqlContext.read.parquet("orders0314_par")
-sqlContext.setConf("spark.sql.parquet.compression.codec","gzip")
-df.write.parquet("orders0314_par_gzip_output")
-or
-sqlContext.setConf("spark.sql.parquet.compression.codec", "snappy")
-df.write.parquet("orders0314_par_snappy_output")
 </t>
   </si>
   <si>
@@ -214,12 +181,157 @@
 sqlContext.setConf("spark.sql.parquet.compression.codec", "snappy")
 df.write.parquet("orders0314_par_snappy_output")</t>
   </si>
+  <si>
+    <t>PARQUET FILE
+(Based on DataFrame)</t>
+  </si>
+  <si>
+    <t>SEQUENCE FILE
+(Class for &lt;K, V&gt;)</t>
+  </si>
+  <si>
+    <t>AVRO FILE
+(Based on DataFrame)</t>
+  </si>
+  <si>
+    <t>JSON FILE
+(Based on DataFrame)</t>
+  </si>
+  <si>
+    <r>
+      <t>TEXT FILE
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Based on RDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">productsRDD.saveAsTextFile("productsRDD")
+hdfs dfs -ls productsRDD
+hdfs dfs -copyToLocal productsRDD/* /home/….
+productsRDD.saveAsTextFile("productsRDD_gzip", </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>classOf[org.apache.hadoop.io.compress.SnappyCodec]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sqlContext.read.parquet("orders0314_par")
+sqlContext.setConf("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spark.sql.parquet.compression.codec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>","gzip")
+df.write.parquet("orders0314_par_gzip_output")
+or
+sqlContext.setConf("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spark.sql.parquet.compression.codec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">", "snappy")
+df.write.parquet("orders0314_par_snappy_output")
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sqlContext.setConf("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spark.sql.avro.compression.codec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>","snappy")
+ordersDF.write.avro("orders_result_snappy")</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +380,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -289,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -350,12 +468,155 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -363,70 +624,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -744,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,233 +1043,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" ht="55.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="D20" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="31"/>
+      <c r="B21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4" ht="55.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="C21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="11" t="s">
+      <c r="D21" s="33" t="s">
         <v>24</v>
-      </c>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
@@ -992,11 +1283,12 @@
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" tooltip="class in org.apache.hadoop.io.compress" display="https://hadoop.apache.org/docs/r3.0.0-alpha2/api/org/apache/hadoop/io/compress/BZip2Codec.html"/>

</xml_diff>